<commit_message>
Updated descriptions of test results for 1-14-2022
</commit_message>
<xml_diff>
--- a/testing_results.XLSX
+++ b/testing_results.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua\Documents\GitHub\JI_Thesis_2021-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF57FC0-1106-4A51-B9C5-6ECC0D4B9458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B5DBA3-7D20-4333-856B-1B6CE3E4A615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Test</t>
   </si>
@@ -76,16 +76,43 @@
   </si>
   <si>
     <t>RAM Used (GB, Approx.)</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-18 NHANES Questionnaire Data </t>
+  </si>
+  <si>
+    <t>Dimensions</t>
+  </si>
+  <si>
+    <t>19643 x 1011</t>
+  </si>
+  <si>
+    <t>19644 x 1011</t>
+  </si>
+  <si>
+    <t>19642 x 1011</t>
+  </si>
+  <si>
+    <t>* default method is stochastic, while 'cart' is not</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -397,24 +424,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E10:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="3" width="55.5546875" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.44140625" customWidth="1"/>
-    <col min="8" max="8" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="55.5546875" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.44140625" customWidth="1"/>
+    <col min="10" max="10" width="20.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -422,73 +449,101 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44575</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44575</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44575</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4">
         <v>3.4</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Code and Results for MICE and parlMICE Runs
</commit_message>
<xml_diff>
--- a/testing_results.XLSX
+++ b/testing_results.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua\Documents\GitHub\JI_Thesis_2021-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B5DBA3-7D20-4333-856B-1B6CE3E4A615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B272EC7-0EFC-47E9-A8A4-C6C8EC31859A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Test</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Runtime (s)</t>
-  </si>
-  <si>
     <t>Errors?</t>
   </si>
   <si>
@@ -66,15 +63,6 @@
     <t>Failed on or after attempting to impute variable AUQ080</t>
   </si>
   <si>
-    <t>MICE Imputation  on NHANES Questionnaire Data + Demographics- default method</t>
-  </si>
-  <si>
-    <t>MICE Imputation  on NHANES Questionnaire Data + Demographics- method = "cart" (classification &amp; Linear regression)</t>
-  </si>
-  <si>
-    <t>data &lt;- mice(data, m = 5, seed = 2022, method = "cart")</t>
-  </si>
-  <si>
     <t>RAM Used (GB, Approx.)</t>
   </si>
   <si>
@@ -84,19 +72,52 @@
     <t xml:space="preserve">2017-18 NHANES Questionnaire Data </t>
   </si>
   <si>
-    <t>Dimensions</t>
-  </si>
-  <si>
     <t>19643 x 1011</t>
   </si>
   <si>
-    <t>19644 x 1011</t>
-  </si>
-  <si>
     <t>19642 x 1011</t>
   </si>
   <si>
-    <t>* default method is stochastic, while 'cart' is not</t>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>9971 x 97</t>
+  </si>
+  <si>
+    <t>MICE Imputation  on NHANES Questionnaire Data  + Demographics</t>
+  </si>
+  <si>
+    <t>MICE Imputation  on NHANES Questionnaire Data (Diet Behavior &amp; Quality + Demographics), method = "cart" (classification &amp; Linear regression)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runtime </t>
+  </si>
+  <si>
+    <t>6.328955 min</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>data &lt;- mice(data, m = 1, seed = 2022, method = "cart")</t>
+  </si>
+  <si>
+    <t>1. default method is stochastic, while 'cart' is not 2. # of Logged events: 176, 3. WRONG DATASET USED (discovered after running)</t>
+  </si>
+  <si>
+    <t>data &lt;- mice(data, m = 1, seed = 2022, method = "cart)</t>
+  </si>
+  <si>
+    <t>22.45882 min</t>
+  </si>
+  <si>
+    <t># of Logged Events: 587</t>
+  </si>
+  <si>
+    <t>9254 x 91</t>
+  </si>
+  <si>
+    <t>Shape (obs x variables)</t>
   </si>
 </sst>
 </file>
@@ -424,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E10:E11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,28 +470,28 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -478,13 +499,13 @@
         <v>44575</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -492,54 +513,97 @@
         <v>44575</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="J3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44575</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
         <v>23</v>
       </c>
       <c r="J4">
         <v>3.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>44575</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>44575</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testing results for 1-14-2022
</commit_message>
<xml_diff>
--- a/testing_results.XLSX
+++ b/testing_results.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua\Documents\GitHub\JI_Thesis_2021-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B272EC7-0EFC-47E9-A8A4-C6C8EC31859A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B9C97E-EF9D-45A1-AEAB-4F871DDC0DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>Test</t>
   </si>
@@ -51,9 +51,6 @@
     <t xml:space="preserve">k-NN with total NHANES Questionnaire data + Demographics- </t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>data &lt;- mice(data, m = 5, seed = 2022)</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>data &lt;- mice(data, m = 1, seed = 2022, method = "cart")</t>
   </si>
   <si>
-    <t>1. default method is stochastic, while 'cart' is not 2. # of Logged events: 176, 3. WRONG DATASET USED (discovered after running)</t>
-  </si>
-  <si>
     <t>data &lt;- mice(data, m = 1, seed = 2022, method = "cart)</t>
   </si>
   <si>
@@ -118,6 +112,24 @@
   </si>
   <si>
     <t>Shape (obs x variables)</t>
+  </si>
+  <si>
+    <t>Function Code</t>
+  </si>
+  <si>
+    <t>combined &lt;- parlmice(combined, m = 5, seed = 2022, method = "cart", n.core = 7, n.imp.core = 2, cluster.seed = 1995)</t>
+  </si>
+  <si>
+    <t>7 cores used, 2 imputations per core. Cluster.seed and seed help ensure reproducibility</t>
+  </si>
+  <si>
+    <t>9255 x 91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. default method is stochastic, while 'cart' is not 2. # of Logged events: 176, </t>
+  </si>
+  <si>
+    <t>WRONG DATASET USED (non-computational, discovered after running)</t>
   </si>
 </sst>
 </file>
@@ -447,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,19 +482,19 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>1</v>
@@ -491,7 +503,7 @@
         <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -502,10 +514,13 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="J2">
+        <v>1.5</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -513,25 +528,25 @@
         <v>44575</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
       </c>
       <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>6</v>
@@ -540,33 +555,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44575</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" t="s">
-        <v>23</v>
+        <v>33</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="J4">
         <v>3.4</v>
@@ -577,33 +592,54 @@
         <v>44575</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>28</v>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5">
+        <v>3.4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44575</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'performance' spreadsheet and runtime results for Random Forest, SVM, Decision Tree, Logistic Regression, LASSO
</commit_message>
<xml_diff>
--- a/testing_results.XLSX
+++ b/testing_results.XLSX
@@ -8,24 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua\Documents\GitHub\JI_Thesis_2021-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B9C97E-EF9D-45A1-AEAB-4F871DDC0DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FD2082-E38F-43A6-9689-5EC12CDDC5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Runtime (Can I run it)" sheetId="1" r:id="rId1"/>
+    <sheet name="Model Performance (ROC)" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="67">
   <si>
     <t>Test</t>
   </si>
@@ -114,29 +124,148 @@
     <t>Shape (obs x variables)</t>
   </si>
   <si>
-    <t>Function Code</t>
-  </si>
-  <si>
     <t>combined &lt;- parlmice(combined, m = 5, seed = 2022, method = "cart", n.core = 7, n.imp.core = 2, cluster.seed = 1995)</t>
   </si>
   <si>
-    <t>7 cores used, 2 imputations per core. Cluster.seed and seed help ensure reproducibility</t>
-  </si>
-  <si>
-    <t>9255 x 91</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. default method is stochastic, while 'cart' is not 2. # of Logged events: 176, </t>
-  </si>
-  <si>
-    <t>WRONG DATASET USED (non-computational, discovered after running)</t>
+    <t>20.4385 min</t>
+  </si>
+  <si>
+    <t>2017-18 NHANES Questionnaire Data (Diet Behavior &amp; Quality + Demographics)</t>
+  </si>
+  <si>
+    <t>9254 x 46</t>
+  </si>
+  <si>
+    <t>MICE Imputation  on NHANES Questionnaire Data (DBQ Question CBQ596 + Demographics), method = "cart" (classification &amp; Linear regression)</t>
+  </si>
+  <si>
+    <t>2017-18 NHANES Questionnaire Data (CBQ596 + Demographics)</t>
+  </si>
+  <si>
+    <t>7.265174 min</t>
+  </si>
+  <si>
+    <t># Of Logged Events: 177</t>
+  </si>
+  <si>
+    <t>combined_mice &lt;- mice(combined, m = 5, seed = 2022, method = "cart")</t>
+  </si>
+  <si>
+    <t>rf_combined &lt;- train(model_recipe, data = data_train, method = model_type, trControl = trControl, metric = 'ROC')</t>
+  </si>
+  <si>
+    <t>Time-Tested Code</t>
+  </si>
+  <si>
+    <t>Variables with &gt; 70% missing after imputation were removed. Mice.complete() was used to retrieve the imputed dataset.</t>
+  </si>
+  <si>
+    <t>2.22736 min</t>
+  </si>
+  <si>
+    <t>1.732804 min</t>
+  </si>
+  <si>
+    <t>Repeat of previous test. Parallelization (via parallel package) was not active during this run</t>
+  </si>
+  <si>
+    <t>rf_combined &lt;- train(model_recipe, data = data_train, method = model_type, trControl = trControl, tGrid = tGrid, metric = 'ROC')</t>
+  </si>
+  <si>
+    <t>3.611931 mins</t>
+  </si>
+  <si>
+    <t>Random Forest on MICE imputed dataset (mice.parlmice())</t>
+  </si>
+  <si>
+    <t>Random Forest on MICE imputed dataset (mice.mice())</t>
+  </si>
+  <si>
+    <t>9254 x 44</t>
+  </si>
+  <si>
+    <t>SVM on MICE imputed dataset (mice.parlmice())</t>
+  </si>
+  <si>
+    <t>svm_combined &lt;- train(model_recipe, data = data_train, method = model_type, trControl = trControl, tuneGrid = tGrid, metric = 'ROC')</t>
+  </si>
+  <si>
+    <r>
+      <t>tGrid &lt;- expand.grid(mtry = c(1:25)) -</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> iterates tuning parameter mtry from 1 to 25</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>tGrid &lt;- expand.grid(C = c(0.001, 0.01, 0.1, 1,5,10,50))</t>
+  </si>
+  <si>
+    <t>WRONG DATASET USED (human error, discovered after running code)</t>
+  </si>
+  <si>
+    <t>1. default method is stochastic, while 'cart' is not 2. # of Logged events: 176</t>
+  </si>
+  <si>
+    <t>7 cores used, 2 imputations per core. Cluster.seed and seed help control for randomness in model when repeated</t>
+  </si>
+  <si>
+    <t>58.79753 mins</t>
+  </si>
+  <si>
+    <t>Logistic Regression on MICE imputed dataset (mice.parlmice())</t>
+  </si>
+  <si>
+    <t>logReg_combined = train(model_recipe, data= data_train, method = model_type, trControl = trControl, tuneLength = 10)</t>
+  </si>
+  <si>
+    <t>5.277871 secs</t>
+  </si>
+  <si>
+    <t>LASSO Regression on MICE imputed dataset (mice.parlmice())</t>
+  </si>
+  <si>
+    <t>lasso_combined &lt;- train(model_recipe, data = data_train, method = model_type, trControl = trControl, tuneGrid = tGrid, metric = "ROC")</t>
+  </si>
+  <si>
+    <t>12.31558 secs</t>
+  </si>
+  <si>
+    <t>tGrid &lt;- expand.grid(alpha = c(1), lambda = 10^seq(1, -2, length = 100))</t>
+  </si>
+  <si>
+    <t>Decision Tree on MICE imputed dataset (mice.parlmice())</t>
+  </si>
+  <si>
+    <t>decisionTree_combined &lt;- train(model_recipe, data = data_train, method = model_type, trControl = trControl, metric = 'ROC', tuneLength = 10)</t>
+  </si>
+  <si>
+    <t>4.449098 secs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +275,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -457,16 +594,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="5" width="55.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" style="1" customWidth="1"/>
+    <col min="2" max="4" width="55.5546875" customWidth="1"/>
+    <col min="5" max="5" width="119.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.44140625" customWidth="1"/>
     <col min="8" max="8" width="24.6640625" style="2" bestFit="1" customWidth="1"/>
@@ -475,7 +613,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
@@ -488,7 +626,7 @@
         <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -519,6 +657,12 @@
       <c r="D2" t="s">
         <v>15</v>
       </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
       <c r="J2">
         <v>1.5</v>
       </c>
@@ -563,7 +707,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -578,10 +722,10 @@
         <v>21</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="J4">
         <v>3.4</v>
@@ -595,7 +739,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
         <v>27</v>
@@ -619,7 +763,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44575</v>
       </c>
@@ -627,23 +771,298 @@
         <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>31</v>
+        <v>55</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="J6">
         <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>44576</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>44576</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>44577</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>44577</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>44577</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <f ca="1">TODAY()</f>
+        <v>44577</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <f ca="1">TODAY()</f>
+        <v>44577</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <f ca="1">TODAY()</f>
+        <v>44577</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14">
+        <v>1.1000000000000001</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B8D9500-B7E3-4A7E-90B6-504B0D1AC0EB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>